<commit_message>
minor changes for brackets email and template
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Bracket_Invoice.xlsx
+++ b/application/controllers/excel-templates/Bracket_Invoice.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>{invoice:invoice_type}</t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>{invoice:19_24_unit_price}</t>
-  </si>
-  <si>
-    <t>{invoice:t19_24_unit_price}</t>
   </si>
   <si>
     <t>{invoice:_26_32_total}</t>
@@ -166,13 +163,19 @@
   </si>
   <si>
     <t>Iron Stand - 15 Inches</t>
+  </si>
+  <si>
+    <t>{invoice:t_19_24_unit_price}</t>
+  </si>
+  <si>
+    <t>{invoice:sub_total}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -215,6 +218,18 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -429,10 +444,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -458,128 +475,127 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -858,7 +874,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -887,169 +903,169 @@
     </row>
     <row r="2" spans="1:9" ht="24" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="15" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="18"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="12"/>
     </row>
     <row r="3" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="21"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="15"/>
     </row>
     <row r="4" spans="1:9" ht="19" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="21"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="15"/>
     </row>
     <row r="5" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20" t="s">
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="23"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="21"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="15"/>
     </row>
     <row r="6" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="23"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="21"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="15"/>
     </row>
     <row r="7" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
       <c r="F7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="23"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="21"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="15"/>
     </row>
     <row r="8" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
       <c r="F8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="23"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="21"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="15"/>
     </row>
     <row r="9" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="1"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="21"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="15"/>
     </row>
     <row r="10" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="26"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="28" t="s">
+      <c r="C10" s="20"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="23"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="21"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="15"/>
     </row>
     <row r="11" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
       <c r="F11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="23"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="21"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="15"/>
     </row>
     <row r="12" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="23"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="21"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="17"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="15"/>
     </row>
     <row r="13" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="1"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="21"/>
+      <c r="B13" s="46"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="15"/>
     </row>
     <row r="14" spans="1:9" ht="28" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="23" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -1062,154 +1078,154 @@
         <v>17</v>
       </c>
       <c r="F14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="H14" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="I14" s="24" t="s">
         <v>38</v>
-      </c>
-      <c r="I14" s="32" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1"/>
-      <c r="B15" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="33">
+      <c r="B15" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="25">
         <v>5</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="34" t="s">
+      <c r="E15" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="21"/>
+      <c r="F15" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="15"/>
     </row>
     <row r="16" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
-      <c r="B16" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="33">
+      <c r="B16" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="25">
         <v>5</v>
       </c>
-      <c r="D16" s="35" t="s">
+      <c r="D16" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="34" t="s">
+      <c r="F16" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="21"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="15"/>
     </row>
     <row r="17" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1"/>
-      <c r="B17" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="33">
+      <c r="B17" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="25">
         <v>5</v>
       </c>
       <c r="D17" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="34" t="s">
+      <c r="F17" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F17" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="21"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="15"/>
     </row>
     <row r="18" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="1"/>
-      <c r="B18" s="36"/>
+      <c r="B18" s="27"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
-      <c r="I18" s="37"/>
+      <c r="I18" s="28"/>
     </row>
     <row r="19" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="1"/>
-      <c r="B19" s="31" t="s">
-        <v>27</v>
+      <c r="B19" s="23" t="s">
+        <v>26</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="38" t="s">
-        <v>28</v>
+      <c r="F19" s="29" t="s">
+        <v>27</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="39"/>
+      <c r="I19" s="30"/>
     </row>
     <row r="20" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="1"/>
-      <c r="B20" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="33">
+      <c r="B20" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="25">
         <v>5</v>
       </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
       <c r="F20" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="21"/>
+        <v>28</v>
+      </c>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="15"/>
     </row>
     <row r="21" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A21" s="1"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="21"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="15"/>
     </row>
     <row r="22" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="1"/>
-      <c r="B22" s="40" t="s">
-        <v>30</v>
+      <c r="B22" s="31" t="s">
+        <v>29</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
-      <c r="F22" s="48" t="s">
-        <v>31</v>
+      <c r="F22" s="38" t="s">
+        <v>45</v>
       </c>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
-      <c r="I22" s="41"/>
+      <c r="I22" s="32"/>
     </row>
     <row r="23" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="1"/>
-      <c r="B23" s="42" t="s">
-        <v>32</v>
+      <c r="B23" s="33" t="s">
+        <v>31</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -1217,48 +1233,48 @@
       <c r="F23" s="6"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
-      <c r="I23" s="43" t="s">
-        <v>31</v>
+      <c r="I23" s="34" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A24" s="1"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="21"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="15"/>
     </row>
     <row r="25" spans="1:9" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
-      <c r="B25" s="44" t="s">
+      <c r="B25" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="D25" s="45"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="45"/>
-      <c r="G25" s="45"/>
-      <c r="H25" s="46"/>
-      <c r="I25" s="47"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="43"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="37"/>
     </row>
     <row r="26" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A26" s="1"/>
-      <c r="B26" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
+      <c r="B26" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1268,5 +1284,6 @@
     <mergeCell ref="B12:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Misc changes in Invoice templates
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Bracket_Invoice.xlsx
+++ b/application/controllers/excel-templates/Bracket_Invoice.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="28560" windowHeight="16400" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,9 +77,6 @@
     <t>Tax %</t>
   </si>
   <si>
-    <t>Quantity</t>
-  </si>
-  <si>
     <t>Rate</t>
   </si>
   <si>
@@ -169,6 +166,9 @@
   </si>
   <si>
     <t>{invoice:sub_total}</t>
+  </si>
+  <si>
+    <t>Units</t>
   </si>
 </sst>
 </file>
@@ -245,7 +245,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -437,6 +437,43 @@
       <right/>
       <top style="thin">
         <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color auto="1"/>
@@ -449,7 +486,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -460,12 +497,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -520,50 +551,59 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -874,7 +914,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -883,7 +923,7 @@
     <col min="2" max="2" width="28.6640625" style="2" customWidth="1"/>
     <col min="3" max="4" width="8.1640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="10" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="6.83203125" style="2" customWidth="1"/>
     <col min="7" max="7" width="8.83203125" style="2" customWidth="1"/>
     <col min="8" max="8" width="8.33203125" style="2" customWidth="1"/>
     <col min="9" max="9" width="10" style="2" customWidth="1"/>
@@ -903,378 +943,378 @@
     </row>
     <row r="2" spans="1:9" ht="24" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="41" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="12"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="15"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="13"/>
     </row>
     <row r="4" spans="1:9" ht="19" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="15"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14" t="s">
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="13"/>
     </row>
     <row r="6" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14" t="s">
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="17"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="13"/>
     </row>
     <row r="7" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="8" t="s">
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="17"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="13"/>
     </row>
     <row r="8" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="8" t="s">
+      <c r="B8" s="17"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="13"/>
     </row>
     <row r="9" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="1"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="15"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="13"/>
     </row>
     <row r="10" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="22" t="s">
+      <c r="C10" s="18"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="17"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="13"/>
     </row>
     <row r="11" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="8" t="s">
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="13"/>
     </row>
     <row r="12" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12" s="17"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="15"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="15"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="13"/>
     </row>
     <row r="13" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="1"/>
-      <c r="B13" s="46"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="15"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="13"/>
     </row>
     <row r="14" spans="1:9" ht="28" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="H14" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="I14" s="39" t="s">
         <v>37</v>
-      </c>
-      <c r="I14" s="24" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1"/>
-      <c r="B15" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="25">
+      <c r="B15" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="22">
         <v>5</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="15"/>
+      <c r="F15" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="13"/>
     </row>
     <row r="16" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
-      <c r="B16" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="25">
+      <c r="B16" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="22">
         <v>5</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="F16" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F16" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="15"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="13"/>
     </row>
     <row r="17" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1"/>
-      <c r="B17" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="25">
+      <c r="B17" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="22">
         <v>5</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="F17" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="15"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="13"/>
     </row>
     <row r="18" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="1"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="28"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="25"/>
     </row>
     <row r="19" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="1"/>
-      <c r="B19" s="23" t="s">
-        <v>26</v>
+      <c r="B19" s="21" t="s">
+        <v>25</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="29" t="s">
-        <v>27</v>
+      <c r="F19" s="26" t="s">
+        <v>26</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="30"/>
+      <c r="I19" s="27"/>
     </row>
     <row r="20" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="1"/>
-      <c r="B20" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="25">
+      <c r="B20" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="22">
         <v>5</v>
       </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="15"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="13"/>
     </row>
     <row r="21" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A21" s="1"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="15"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="13"/>
     </row>
     <row r="22" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="1"/>
-      <c r="B22" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="32"/>
+      <c r="B22" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="29"/>
     </row>
     <row r="23" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="1"/>
-      <c r="B23" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="34" t="s">
+      <c r="B23" s="30" t="s">
         <v>30</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="31" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A24" s="1"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="15"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="13"/>
     </row>
     <row r="25" spans="1:9" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
-      <c r="B25" s="35" t="s">
+      <c r="B25" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="43"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="37"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="34"/>
     </row>
     <row r="26" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A26" s="1"/>
-      <c r="B26" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
-      <c r="F26" s="40"/>
-      <c r="G26" s="40"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="40"/>
+      <c r="B26" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="41"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
+      <c r="G26" s="41"/>
+      <c r="H26" s="41"/>
+      <c r="I26" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>